<commit_message>
docs: API 문서 수정
- 상품목록가져오기의 pData를 씌우지 않음
</commit_message>
<xml_diff>
--- a/설계/01. 화면정의서/API_List.xlsx
+++ b/설계/01. 화면정의서/API_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NewProject\ESupply\설계\01. 화면정의서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\자유연습\ESupply\설계\01. 화면정의서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40CCA37-21E2-4AC4-AA2C-57894D8A436B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7B8116-E33B-4AB8-9B54-39F81F83BE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF6AAFE8-485D-4D85-8366-6D2DAC35A2AB}"/>
   </bookViews>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -244,15 +235,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{ 
-    pData :  { 
-       count : 108, 
-       pList   : [ { product_nm : "aaaaa", product_id : "cap_2349809", count : 100 , image : "" }, …. ]
-    }
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{
     pData : { [  { part_no, part_nm, price, weight, size_h, size_v, size_z, count, image}, {…}, ...
     ] }
@@ -262,6 +244,13 @@
   <si>
     <t>{
     pData : { part_no, part_nm, price, weight, size_h, size_v, size_z, count, image }
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{     
+     count : 108, 
+     pList   : [ { product_nm : "aaaaa", product_id : "cap_2349809", count : 100 , image : "" }, …. ]
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -671,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553ED3CF-FB64-48E3-BACA-99279F6927A6}">
   <dimension ref="B1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -735,7 +724,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="66" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -749,7 +738,7 @@
         <v>35</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="231" x14ac:dyDescent="0.3">
@@ -811,7 +800,7 @@
         <v>38</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
@@ -826,7 +815,7 @@
         <v>40</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: API_LIST 상품등록 추가
</commit_message>
<xml_diff>
--- a/설계/01. 화면정의서/API_List.xlsx
+++ b/설계/01. 화면정의서/API_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\자유연습\ESupply\설계\01. 화면정의서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7B8116-E33B-4AB8-9B54-39F81F83BE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855F8FA7-554C-4297-9204-35C0F09752F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF6AAFE8-485D-4D85-8366-6D2DAC35A2AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF6AAFE8-485D-4D85-8366-6D2DAC35A2AB}"/>
   </bookViews>
   <sheets>
     <sheet name="(주)선아전자" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>로그인시도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,6 +251,38 @@
     <t>{     
      count : 108, 
      pList   : [ { product_nm : "aaaaa", product_id : "cap_2349809", count : 100 , image : "" }, …. ]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGadd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/product/add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "class_id" : "DIO_120",
+    "product_id" : "DIO_120_DLCGBB999340",
+    "product_nm" : "광다이오드_120",
+    "price" : "950",
+    "weight" : "90",
+    "size_h" : "62",
+    "size_v" : "22",
+    "size_z" : "22"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    count : 1,
+    result : "Success"
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -658,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553ED3CF-FB64-48E3-BACA-99279F6927A6}">
-  <dimension ref="B1:F21"/>
+  <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -741,114 +773,124 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="231" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="165" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="231" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" ht="66" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="2:6" ht="66" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="2:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
@@ -914,6 +956,13 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ESupply - Swagger 적용완료  API /product/gooddel  requestbody 수정
</commit_message>
<xml_diff>
--- a/설계/01. 화면정의서/API_List.xlsx
+++ b/설계/01. 화면정의서/API_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NewProject\ESupply\설계\01. 화면정의서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B9DE47-9AF2-493F-9F63-4AA327B1BAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47D9502-B37B-4745-92FC-1B13F274468B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,20 +507,22 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>/part/list</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ 
+    product_id : "aaaaa",            // 제품ID
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>{ 
     class_id
     product_id
     serial_no 
-}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>/part/list</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{ 
-    product_id : "aaaaa",            // 제품ID
+    out_type                // 출고 구분("DISPOSE", "SALE")
+    order_no                // 주문번호(출고구분이 "SALE" 일때 필수입력)
 }</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1047,7 +1049,7 @@
   <dimension ref="B1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1208,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B10" s="21" t="s">
         <v>120</v>
       </c>
@@ -1216,8 +1218,8 @@
       <c r="D10" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>126</v>
+      <c r="E10" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>124</v>
@@ -1276,10 +1278,10 @@
         <v>51</v>
       </c>
       <c r="D14" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
esupply - api 수정
</commit_message>
<xml_diff>
--- a/설계/01. 화면정의서/API_List.xlsx
+++ b/설계/01. 화면정의서/API_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NewProject\ESupply\설계\01. 화면정의서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47D9502-B37B-4745-92FC-1B13F274468B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB7CA72-1969-4494-8530-141FD074EAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,7 +1049,7 @@
   <dimension ref="B1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>